<commit_message>
Fixed some bugs with import/export
</commit_message>
<xml_diff>
--- a/Presentation.Web/Content/mox/OS2KITOS MOX Skabelon Organisation.xlsx
+++ b/Presentation.Web/Content/mox/OS2KITOS MOX Skabelon Organisation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="24915" windowHeight="12015" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="24915" windowHeight="12015" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Parametre" sheetId="3" r:id="rId1"/>
@@ -1151,8 +1151,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1784,7 +1784,7 @@
   <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B484"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5101,7 +5101,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
@@ -5330,27 +5330,27 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Rolle!$A$8:$A$42</xm:f>
-          </x14:formula1>
-          <xm:sqref>C9:C134</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>Bruger!$B$8:$B$136</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D677</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Rolle!$C$8:$C$18</xm:f>
+            <xm:f>Organisation!$C$41:$C$595</xm:f>
           </x14:formula1>
-          <xm:sqref>C8</xm:sqref>
+          <xm:sqref>B8:B9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Organisation!$C$41:$C$595</xm:f>
+            <xm:f>Rolle!$A$8:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>B8:B9</xm:sqref>
+          <xm:sqref>C9:C134</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Rolle!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>C8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5363,7 +5363,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D22"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
@@ -5567,10 +5567,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5655,99 +5655,6 @@
       <c r="B7" s="61"/>
       <c r="C7" s="61"/>
     </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5759,7 +5666,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E2167"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5861,8 +5768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>